<commit_message>
updated retriever eval results xlsx
</commit_message>
<xml_diff>
--- a/src/tests/retriever_eval.xlsx
+++ b/src/tests/retriever_eval.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,29 +488,29 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': True, 'trust_remote_code': True}</t>
+          <t>{'instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'query_instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'load_in_8bit': True, 'trust_remote_code': True}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>67.69</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>72.31</v>
+        <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>76.92</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>81.54000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alibaba-NLP/gte-Qwen2-1.5B-instruct</t>
+          <t>dunzhang/stella_en_1.5B_v5</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,29 +520,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': True}</t>
+          <t>{'instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'query_instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'load_in_8bit': False, 'trust_remote_code': True}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>21.54</v>
+        <v>95.38</v>
       </c>
       <c r="E3" t="n">
-        <v>30.77</v>
+        <v>96.92</v>
       </c>
       <c r="F3" t="n">
-        <v>38.46</v>
+        <v>96.92</v>
       </c>
       <c r="G3" t="n">
-        <v>41.54</v>
+        <v>96.92</v>
       </c>
       <c r="H3" t="n">
-        <v>41.54</v>
+        <v>96.92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alibaba-NLP/gte-Qwen2-1.5B-instruct</t>
+          <t>sentence-transformers/all-MiniLM-L6-v2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -552,29 +552,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
+          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>16.92</v>
+        <v>78.45999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>29.23</v>
+        <v>89.23</v>
       </c>
       <c r="F4" t="n">
-        <v>35.38</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="G4" t="n">
-        <v>44.62</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>47.69</v>
+        <v>93.84999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alibaba-NLP/gte-Qwen2-1.5B-instruct</t>
+          <t>MSMARCO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -584,29 +584,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': True, 'trust_remote_code': False}</t>
+          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>15.38</v>
+        <v>69.23</v>
       </c>
       <c r="E5" t="n">
-        <v>29.23</v>
+        <v>84.62</v>
       </c>
       <c r="F5" t="n">
-        <v>35.38</v>
+        <v>89.23</v>
       </c>
       <c r="G5" t="n">
-        <v>46.15</v>
+        <v>90.77</v>
       </c>
       <c r="H5" t="n">
-        <v>47.69</v>
+        <v>90.77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dunzhang/stella_en_1.5B_v5</t>
+          <t>mxbai embed large</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -616,343 +616,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
+          <t>{'instruction': 'Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>43.08</v>
+        <v>86.15000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>47.69</v>
+        <v>90.77</v>
       </c>
       <c r="F6" t="n">
-        <v>50.77</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>60</v>
+        <v>93.84999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>61.54</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>dunzhang/stella_en_1.5B_v5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': True}</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>90.77</v>
-      </c>
-      <c r="E7" t="n">
-        <v>96.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>98.45999999999999</v>
-      </c>
-      <c r="G7" t="n">
-        <v>98.45999999999999</v>
-      </c>
-      <c r="H7" t="n">
-        <v>98.45999999999999</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sentence-transformers/all-MiniLM-L6-v2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>58.46</v>
-      </c>
-      <c r="E8" t="n">
-        <v>73.84999999999999</v>
-      </c>
-      <c r="F8" t="n">
-        <v>76.92</v>
-      </c>
-      <c r="G8" t="n">
-        <v>83.08</v>
-      </c>
-      <c r="H8" t="n">
-        <v>86.15000000000001</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sentence-transformers/all-MiniLM-L6-v2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': True}</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>58.46</v>
-      </c>
-      <c r="E9" t="n">
-        <v>73.84999999999999</v>
-      </c>
-      <c r="F9" t="n">
-        <v>76.92</v>
-      </c>
-      <c r="G9" t="n">
-        <v>83.08</v>
-      </c>
-      <c r="H9" t="n">
-        <v>86.15000000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>BioBERT</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>10.77</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12.31</v>
-      </c>
-      <c r="F10" t="n">
-        <v>18.46</v>
-      </c>
-      <c r="G10" t="n">
-        <v>18.46</v>
-      </c>
-      <c r="H10" t="n">
-        <v>18.46</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>BERT Base Uncased</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>16.92</v>
-      </c>
-      <c r="E11" t="n">
-        <v>21.54</v>
-      </c>
-      <c r="F11" t="n">
-        <v>26.15</v>
-      </c>
-      <c r="G11" t="n">
-        <v>30.77</v>
-      </c>
-      <c r="H11" t="n">
-        <v>32.31</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>RoBERTa Base</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.62</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6.15</v>
-      </c>
-      <c r="G12" t="n">
-        <v>6.15</v>
-      </c>
-      <c r="H12" t="n">
-        <v>9.23</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>RoBERTa Large</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>9.23</v>
-      </c>
-      <c r="E13" t="n">
-        <v>18.46</v>
-      </c>
-      <c r="F13" t="n">
-        <v>27.69</v>
-      </c>
-      <c r="G13" t="n">
-        <v>30.77</v>
-      </c>
-      <c r="H13" t="n">
-        <v>35.38</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>BERT Large NLI</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>41.54</v>
-      </c>
-      <c r="E14" t="n">
-        <v>46.15</v>
-      </c>
-      <c r="F14" t="n">
-        <v>50.77</v>
-      </c>
-      <c r="G14" t="n">
-        <v>53.85</v>
-      </c>
-      <c r="H14" t="n">
-        <v>55.38</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>MSMARCO</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>47.69</v>
-      </c>
-      <c r="E15" t="n">
-        <v>64.62</v>
-      </c>
-      <c r="F15" t="n">
-        <v>72.31</v>
-      </c>
-      <c r="G15" t="n">
-        <v>78.45999999999999</v>
-      </c>
-      <c r="H15" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>mxbai embed large</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>hf://datasets/m-ric/huggingface_doc_qa_eval/data/train-00000-of-00001.parquet</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>{'instruction': 'Instruct: Given a technical query, find the most relevant passages that can provide the answer.\nPassage:', 'query_instruction': 'Instruct: Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'load_in_8bit': False, 'trust_remote_code': False}</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>21.54</v>
-      </c>
-      <c r="E16" t="n">
-        <v>23.08</v>
-      </c>
-      <c r="F16" t="n">
-        <v>23.08</v>
-      </c>
-      <c r="G16" t="n">
-        <v>23.08</v>
-      </c>
-      <c r="H16" t="n">
-        <v>23.08</v>
+        <v>93.84999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated eval results excel files with all models
</commit_message>
<xml_diff>
--- a/src/tests/retriever_eval.xlsx
+++ b/src/tests/retriever_eval.xlsx
@@ -492,19 +492,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>93.84999999999999</v>
+        <v>92.31</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>98.45999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>95.38</v>
+        <v>92.31</v>
       </c>
       <c r="E3" t="n">
         <v>96.92</v>
@@ -556,25 +556,25 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>78.45999999999999</v>
+        <v>64.62</v>
       </c>
       <c r="E4" t="n">
-        <v>89.23</v>
+        <v>75.38</v>
       </c>
       <c r="F4" t="n">
-        <v>93.84999999999999</v>
+        <v>80</v>
       </c>
       <c r="G4" t="n">
-        <v>93.84999999999999</v>
+        <v>81.54000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>93.84999999999999</v>
+        <v>81.54000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MSMARCO</t>
+          <t>mixedbread-ai/mxbai-embed-large-v1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -588,25 +588,25 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>69.23</v>
+        <v>87.69</v>
       </c>
       <c r="E5" t="n">
-        <v>84.62</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="F5" t="n">
-        <v>89.23</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>90.77</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>90.77</v>
+        <v>98.45999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mxbai embed large</t>
+          <t>MSMARCO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -616,23 +616,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'instruction': 'Represent this passage for retrieval in response to relevant technical questions.\nQuery:', 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
+          <t>{'instruction': None, 'query_instruction': None, 'load_in_8bit': False, 'trust_remote_code': False}</t>
         </is>
       </c>
       <c r="D6" t="n">
+        <v>76.92</v>
+      </c>
+      <c r="E6" t="n">
         <v>86.15000000000001</v>
       </c>
-      <c r="E6" t="n">
-        <v>90.77</v>
-      </c>
       <c r="F6" t="n">
-        <v>93.84999999999999</v>
+        <v>87.69</v>
       </c>
       <c r="G6" t="n">
-        <v>93.84999999999999</v>
+        <v>89.23</v>
       </c>
       <c r="H6" t="n">
-        <v>93.84999999999999</v>
+        <v>89.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>